<commit_message>
Bulk-upload new column added in file format
</commit_message>
<xml_diff>
--- a/public/assets/download-format/bulk_user_upload_v2.xlsx
+++ b/public/assets/download-format/bulk_user_upload_v2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
   <si>
     <t xml:space="preserve">user_first_name</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t xml:space="preserve">sibling_school_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mappingSubject</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
@@ -293,7 +296,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="yyyy/dd/mm;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -323,6 +326,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans Light"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -366,7 +382,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -387,7 +403,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -476,13 +500,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BH4"/>
+  <dimension ref="A1:BI4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BI1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BL17" activeCellId="0" sqref="BL17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="22.01"/>
@@ -522,7 +546,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="18.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="17.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="24.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="25.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="16.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,28 +731,31 @@
       <c r="BH1" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="BI1" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="5" t="n">
+        <v>63</v>
+      </c>
+      <c r="D2" s="6" t="n">
         <v>41187</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>23223</v>
@@ -736,115 +764,115 @@
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>12</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="V2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC2" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="W2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AD2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AN2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="AT2" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AU2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AV2" s="4" t="n">
         <v>145</v>
@@ -856,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AZ2" s="0" t="n">
         <v>1</v>
@@ -865,65 +893,66 @@
         <v>23</v>
       </c>
       <c r="BB2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="BC2" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="BC2" s="0" t="s">
-        <v>85</v>
-      </c>
+      <c r="BI2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="6"/>
+      <c r="D3" s="8"/>
       <c r="W3" s="4"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
       <c r="AC3" s="4"/>
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
       <c r="AL3" s="4"/>
       <c r="AM3" s="4"/>
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
-      <c r="AP3" s="7"/>
-      <c r="AQ3" s="7"/>
-      <c r="AR3" s="7"/>
-      <c r="AS3" s="7"/>
-      <c r="AT3" s="7"/>
+      <c r="AP3" s="9"/>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="9"/>
+      <c r="AS3" s="9"/>
+      <c r="AT3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="6"/>
+      <c r="D4" s="8"/>
       <c r="W4" s="4"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7"/>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="7"/>
+      <c r="AP4" s="9"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="9"/>
+      <c r="AS4" s="9"/>
+      <c r="AT4" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -934,7 +963,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.08263888888889" bottom="1.08263888888889" header="0.886111111111111" footer="0.886111111111111"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>